<commit_message>
BP-1588 category all apis
</commit_message>
<xml_diff>
--- a/assets/courses/Maximum.xlsx
+++ b/assets/courses/Maximum.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Платовская ул, 4</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Профориентация</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -226,6 +232,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -535,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,23 +555,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="48.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14">
+    <row r="1" spans="1:7" ht="14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -569,17 +581,20 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="97" customHeight="1">
+    <row r="2" spans="1:7" ht="97" customHeight="1">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -589,19 +604,22 @@
       <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1">
-      <c r="D8" s="1"/>
+    <row r="8" spans="1:7" ht="17.25" customHeight="1">
       <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>